<commit_message>
fix: update GAS URL to final deployment and clean up debug code
</commit_message>
<xml_diff>
--- a/商品揭露v2.xlsx
+++ b/商品揭露v2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="252">
   <si>
     <t>WaveID</t>
   </si>
@@ -695,9 +695,6 @@
     <t>POPO</t>
   </si>
   <si>
-    <t>【韓國SAM'S】濟州牛島風味夾心餅(綠茶風味),參虎吃不停爆紅薏仁,【韓國SAM'S】濟州牛島風味夾心餅(柑橘風味),【KAO】HAITER浴室泡沫漂白噴霧,義美巧克力小泡芙57g,【LEC超值組】激落君 強力除霉泡泡,【My料理所】日式咖哩牛,統一生機 海鹽洋芋片</t>
-  </si>
-  <si>
     <t>波段</t>
   </si>
   <si>
@@ -780,6 +777,54 @@
   </si>
   <si>
     <t>{"action":"enable_product","wave":"2","leaderId":"Ub6e6a2d6e6358bd68b656638e974b1c6","leaderName":"POPO","prodName":"統一生機 海鹽洋芋片","isEnabled":true}</t>
+  </si>
+  <si>
+    <t>{"leaderId":"DEV_TEST"}</t>
+  </si>
+  <si>
+    <t>{"action":"enable_product","wave":"2","leaderId":"DEV_TEST","leaderName":"測試團購主","prodName":"參虎吃不停爆紅薏仁","isEnabled":true}</t>
+  </si>
+  <si>
+    <t>DEBUG_Toggle</t>
+  </si>
+  <si>
+    <t>{"prodName":"參虎吃不停爆紅薏仁","shouldEnable":true,"bindingKey":"DEV_TEST_2"}</t>
+  </si>
+  <si>
+    <t>{"leaderId":"DEV_TEST","userId":"DEV_TEST"}</t>
+  </si>
+  <si>
+    <t>{"action":"enable_product","wave":"2","leaderId":"DEV_TEST","leaderName":"測試團購主","prodName":"參虎吃不停爆紅薏仁","isEnabled":false}</t>
+  </si>
+  <si>
+    <t>{"prodName":"參虎吃不停爆紅薏仁","shouldEnable":false,"bindingKey":"DEV_TEST_2"}</t>
+  </si>
+  <si>
+    <t>{"action":"enable_product","wave":"2","leaderId":"Ub6e6a2d6e6358bd68b656638e974b1c6","leaderName":"POPO","prodName":"義美巧克力小泡芙57g","isEnabled":false}</t>
+  </si>
+  <si>
+    <t>{"prodName":"參虎吃不停爆紅薏仁","shouldEnable":false,"bindingKey":"Ub6e6a2d6e6358bd68b656638e974b1c6_2"}</t>
+  </si>
+  <si>
+    <t>{"action":"enable_product","wave":"2","leaderId":"Ub6e6a2d6e6358bd68b656638e974b1c6","leaderName":"POPO","prodName":"參虎吃不停爆紅薏仁","isEnabled":true}</t>
+  </si>
+  <si>
+    <t>{"action":"enable_product","wave":"2","leaderId":"Ub6e6a2d6e6358bd68b656638e974b1c6","leaderName":"POPO","prodName":"【韓國SAM'S】濟州牛島風味夾心餅(綠茶風味)","isEnabled":false}</t>
+  </si>
+  <si>
+    <t>{"action":"enable_product","wave":"2","leaderId":"Ub6e6a2d6e6358bd68b656638e974b1c6","leaderName":"POPO","prodName":"【韓國SAM'S】濟州牛島風味夾心餅(柑橘風味)","isEnabled":false}</t>
+  </si>
+  <si>
+    <t>{"action":"enable_product","wave":"2","leaderId":"Ub6e6a2d6e6358bd68b656638e974b1c6","leaderName":"POPO","prodName":"統一生機 海鹽洋芋片","isEnabled":false}</t>
+  </si>
+  <si>
+    <t>{"action":"enable_product","wave":"2","leaderId":"Ub6e6a2d6e6358bd68b656638e974b1c6","leaderName":"POPO","prodName":"【My料理所】日式咖哩牛","isEnabled":false}</t>
+  </si>
+  <si>
+    <t>{"action":"enable_product","wave":"2","leaderId":"Ub6e6a2d6e6358bd68b656638e974b1c6","leaderName":"POPO","prodName":"【KAO】HAITER浴室泡沫漂白噴霧","isEnabled":false}</t>
+  </si>
+  <si>
+    <t>{"action":"enable_product","wave":"2","leaderId":"Ub6e6a2d6e6358bd68b656638e974b1c6","leaderName":"POPO","prodName":"【LEC超值組】激落君 強力除霉泡泡","isEnabled":false}</t>
   </si>
 </sst>
 </file>
@@ -6112,7 +6157,7 @@
         <v>46046.02491177083</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>208</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3">
@@ -9101,30 +9146,30 @@
         <v>198</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>200</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="22" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B2" s="22">
         <v>2.0</v>
@@ -9148,12 +9193,12 @@
         <v>207</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B3" s="22">
         <v>2.0</v>
@@ -9177,12 +9222,12 @@
         <v>207</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="22" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B4" s="22">
         <v>2.0</v>
@@ -9206,12 +9251,12 @@
         <v>207</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="22" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B5" s="22">
         <v>2.0</v>
@@ -9235,12 +9280,12 @@
         <v>207</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="22" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B6" s="22">
         <v>2.0</v>
@@ -9264,7 +9309,7 @@
         <v>207</v>
       </c>
       <c r="I6" s="27" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7">
@@ -9507,13 +9552,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="22" t="s">
+        <v>216</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>217</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="C1" s="22" t="s">
         <v>218</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="2">
@@ -9521,10 +9566,10 @@
         <v>46046.02479954861</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C2" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="3">
@@ -9532,10 +9577,10 @@
         <v>46046.02489238426</v>
       </c>
       <c r="B3" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="4">
@@ -9543,10 +9588,10 @@
         <v>46046.02500162037</v>
       </c>
       <c r="B4" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C4" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="5">
@@ -9554,10 +9599,10 @@
         <v>46046.02504511574</v>
       </c>
       <c r="B5" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C5" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="6">
@@ -9565,10 +9610,10 @@
         <v>46046.026046956016</v>
       </c>
       <c r="B6" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C6" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="7">
@@ -9576,10 +9621,10 @@
         <v>46046.02608243056</v>
       </c>
       <c r="B7" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C7" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="8">
@@ -9587,10 +9632,10 @@
         <v>46046.02637346065</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9">
@@ -9598,10 +9643,10 @@
         <v>46046.026396863424</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10">
@@ -9609,10 +9654,10 @@
         <v>46046.0264075</v>
       </c>
       <c r="B10" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C10" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="11">
@@ -9620,10 +9665,10 @@
         <v>46046.026436898144</v>
       </c>
       <c r="B11" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C11" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="12">
@@ -9631,10 +9676,10 @@
         <v>46046.02645986111</v>
       </c>
       <c r="B12" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C12" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="13">
@@ -9642,10 +9687,10 @@
         <v>46046.02647210648</v>
       </c>
       <c r="B13" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C13" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="14">
@@ -9653,10 +9698,10 @@
         <v>46046.02657628473</v>
       </c>
       <c r="B14" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C14" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="15">
@@ -9664,10 +9709,10 @@
         <v>46046.02662337963</v>
       </c>
       <c r="B15" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C15" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="16">
@@ -9675,10 +9720,10 @@
         <v>46046.02933185185</v>
       </c>
       <c r="B16" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C16" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="17">
@@ -9686,10 +9731,10 @@
         <v>46046.029401921296</v>
       </c>
       <c r="B17" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C17" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="18">
@@ -9697,10 +9742,10 @@
         <v>46046.02976761574</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="19">
@@ -9708,10 +9753,10 @@
         <v>46046.02979935185</v>
       </c>
       <c r="B19" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C19" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="20">
@@ -9719,10 +9764,10 @@
         <v>46046.02983885417</v>
       </c>
       <c r="B20" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C20" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="21">
@@ -9730,10 +9775,10 @@
         <v>46046.032734293985</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="22">
@@ -9741,10 +9786,10 @@
         <v>46046.032772164355</v>
       </c>
       <c r="B22" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C22" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="23">
@@ -9752,10 +9797,10 @@
         <v>46046.032804560185</v>
       </c>
       <c r="B23" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C23" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="24">
@@ -9763,10 +9808,10 @@
         <v>46046.0329852662</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="25">
@@ -9774,10 +9819,10 @@
         <v>46046.033023958335</v>
       </c>
       <c r="B25" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C25" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="26">
@@ -9785,10 +9830,10 @@
         <v>46046.033064664356</v>
       </c>
       <c r="B26" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C26" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="27">
@@ -9796,10 +9841,10 @@
         <v>46046.03317547454</v>
       </c>
       <c r="B27" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C27" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C27" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="28">
@@ -9807,10 +9852,10 @@
         <v>46046.03321385417</v>
       </c>
       <c r="B28" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C28" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C28" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="29">
@@ -9818,10 +9863,10 @@
         <v>46046.03435987269</v>
       </c>
       <c r="B29" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C29" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C29" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="30">
@@ -9829,10 +9874,10 @@
         <v>46046.03439872686</v>
       </c>
       <c r="B30" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C30" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C30" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="31">
@@ -9840,10 +9885,10 @@
         <v>46046.03715984954</v>
       </c>
       <c r="B31" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C31" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C31" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="32">
@@ -9851,10 +9896,10 @@
         <v>46046.03720045139</v>
       </c>
       <c r="B32" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C32" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C32" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="33">
@@ -9862,10 +9907,10 @@
         <v>46046.03785222222</v>
       </c>
       <c r="B33" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C33" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C33" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="34">
@@ -9873,10 +9918,10 @@
         <v>46046.03789633102</v>
       </c>
       <c r="B34" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C34" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C34" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="35">
@@ -9884,10 +9929,10 @@
         <v>46046.04064233796</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="36">
@@ -9895,10 +9940,10 @@
         <v>46046.040680509264</v>
       </c>
       <c r="B36" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C36" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C36" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="37">
@@ -9906,10 +9951,10 @@
         <v>46046.04074384259</v>
       </c>
       <c r="B37" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C37" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C37" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="38">
@@ -9917,10 +9962,10 @@
         <v>46046.04576849537</v>
       </c>
       <c r="B38" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C38" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C38" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="39">
@@ -9928,10 +9973,10 @@
         <v>46046.04580277778</v>
       </c>
       <c r="B39" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C39" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C39" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="40">
@@ -9939,10 +9984,10 @@
         <v>46046.046033125</v>
       </c>
       <c r="B40" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C40" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C40" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="41">
@@ -9950,10 +9995,10 @@
         <v>46046.04609027778</v>
       </c>
       <c r="B41" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C41" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C41" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="42">
@@ -9961,10 +10006,10 @@
         <v>46046.046188865745</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="43">
@@ -9972,10 +10017,10 @@
         <v>46046.04621502315</v>
       </c>
       <c r="B43" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C43" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C43" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="44">
@@ -9983,10 +10028,10 @@
         <v>46046.046249583334</v>
       </c>
       <c r="B44" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C44" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C44" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="45">
@@ -9994,10 +10039,10 @@
         <v>46046.0463518287</v>
       </c>
       <c r="B45" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C45" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C45" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="46">
@@ -10005,10 +10050,10 @@
         <v>46046.04638650463</v>
       </c>
       <c r="B46" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C46" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C46" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="47">
@@ -10016,10 +10061,10 @@
         <v>46046.046469270834</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="48">
@@ -10027,10 +10072,10 @@
         <v>46046.04650615741</v>
       </c>
       <c r="B48" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C48" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C48" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="49">
@@ -10038,10 +10083,10 @@
         <v>46046.04654181713</v>
       </c>
       <c r="B49" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C49" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C49" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="50">
@@ -10049,10 +10094,10 @@
         <v>46046.046614363426</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="51">
@@ -10060,10 +10105,10 @@
         <v>46046.04664215278</v>
       </c>
       <c r="B51" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C51" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C51" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="52">
@@ -10071,10 +10116,10 @@
         <v>46046.04667915509</v>
       </c>
       <c r="B52" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C52" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C52" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="53">
@@ -10082,10 +10127,10 @@
         <v>46046.04682210648</v>
       </c>
       <c r="B53" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="54">
@@ -10093,10 +10138,10 @@
         <v>46046.046857037036</v>
       </c>
       <c r="B54" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C54" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C54" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="55">
@@ -10104,10 +10149,10 @@
         <v>46046.04686969907</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="56">
@@ -10115,10 +10160,10 @@
         <v>46046.04689347222</v>
       </c>
       <c r="B56" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C56" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C56" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="57">
@@ -10126,10 +10171,10 @@
         <v>46046.046928703705</v>
       </c>
       <c r="B57" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C57" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C57" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="58">
@@ -10137,10 +10182,10 @@
         <v>46046.046994965276</v>
       </c>
       <c r="B58" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C58" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C58" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="59">
@@ -10148,10 +10193,10 @@
         <v>46046.05659807871</v>
       </c>
       <c r="B59" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C59" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C59" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="60">
@@ -10159,10 +10204,10 @@
         <v>46046.05663641204</v>
       </c>
       <c r="B60" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C60" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C60" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="61">
@@ -10170,10 +10215,10 @@
         <v>46046.05666674768</v>
       </c>
       <c r="B61" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="62">
@@ -10181,10 +10226,10 @@
         <v>46046.05670078704</v>
       </c>
       <c r="B62" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C62" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C62" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="63">
@@ -10192,10 +10237,10 @@
         <v>46046.0567497338</v>
       </c>
       <c r="B63" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C63" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C63" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="64">
@@ -10203,10 +10248,10 @@
         <v>46046.06126652777</v>
       </c>
       <c r="B64" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C64" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C64" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="65">
@@ -10214,10 +10259,10 @@
         <v>46046.06130425926</v>
       </c>
       <c r="B65" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C65" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C65" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="66">
@@ -10225,10 +10270,10 @@
         <v>46046.06379240741</v>
       </c>
       <c r="B66" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C66" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C66" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="67">
@@ -10236,10 +10281,10 @@
         <v>46046.06382815972</v>
       </c>
       <c r="B67" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C67" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C67" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="68">
@@ -10247,10 +10292,10 @@
         <v>46046.06397108796</v>
       </c>
       <c r="B68" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C68" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C68" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="69">
@@ -10258,10 +10303,10 @@
         <v>46046.06402038195</v>
       </c>
       <c r="B69" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C69" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C69" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="70">
@@ -10269,10 +10314,10 @@
         <v>46046.064113541666</v>
       </c>
       <c r="B70" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C70" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="71">
@@ -10280,10 +10325,10 @@
         <v>46046.064140312505</v>
       </c>
       <c r="B71" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C71" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C71" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="72">
@@ -10291,10 +10336,10 @@
         <v>46046.06418284722</v>
       </c>
       <c r="B72" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C72" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C72" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="73">
@@ -10302,10 +10347,10 @@
         <v>46046.0642878588</v>
       </c>
       <c r="B73" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C73" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C73" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="74">
@@ -10313,10 +10358,10 @@
         <v>46046.064330520836</v>
       </c>
       <c r="B74" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C74" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C74" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="75">
@@ -10324,10 +10369,10 @@
         <v>46046.065409814815</v>
       </c>
       <c r="B75" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C75" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="76">
@@ -10335,10 +10380,10 @@
         <v>46046.06544342593</v>
       </c>
       <c r="B76" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C76" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C76" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="77">
@@ -10346,10 +10391,10 @@
         <v>46046.06548225695</v>
       </c>
       <c r="B77" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C77" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C77" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="78">
@@ -10357,10 +10402,10 @@
         <v>46046.06580803241</v>
       </c>
       <c r="B78" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C78" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C78" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="79">
@@ -10368,10 +10413,10 @@
         <v>46046.06585971065</v>
       </c>
       <c r="B79" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C79" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C79" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="80">
@@ -10379,10 +10424,10 @@
         <v>46046.06661214121</v>
       </c>
       <c r="B80" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C80" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="81">
@@ -10390,10 +10435,10 @@
         <v>46046.066650162036</v>
       </c>
       <c r="B81" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C81" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C81" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="82">
@@ -10401,10 +10446,10 @@
         <v>46046.06668521991</v>
       </c>
       <c r="B82" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C82" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C82" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="83">
@@ -10412,10 +10457,10 @@
         <v>46046.066809710646</v>
       </c>
       <c r="B83" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C83" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C83" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="84">
@@ -10423,10 +10468,10 @@
         <v>46046.066849236115</v>
       </c>
       <c r="B84" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C84" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C84" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="85">
@@ -10434,10 +10479,10 @@
         <v>46046.066881446764</v>
       </c>
       <c r="B85" s="22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C85" s="22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="86">
@@ -10445,10 +10490,10 @@
         <v>46046.066924363426</v>
       </c>
       <c r="B86" s="22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C86" s="22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="87">
@@ -10456,10 +10501,10 @@
         <v>46046.06779958333</v>
       </c>
       <c r="B87" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C87" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C87" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="88">
@@ -10467,10 +10512,10 @@
         <v>46046.06781771991</v>
       </c>
       <c r="B88" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C88" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C88" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="89">
@@ -10478,10 +10523,10 @@
         <v>46046.067858622686</v>
       </c>
       <c r="B89" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C89" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C89" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="90">
@@ -10489,10 +10534,10 @@
         <v>46046.067975439815</v>
       </c>
       <c r="B90" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C90" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C90" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="91">
@@ -10500,10 +10545,10 @@
         <v>46046.06803527778</v>
       </c>
       <c r="B91" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C91" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C91" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="92">
@@ -10511,10 +10556,10 @@
         <v>46046.068119814816</v>
       </c>
       <c r="B92" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C92" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="93">
@@ -10522,10 +10567,10 @@
         <v>46046.068152418986</v>
       </c>
       <c r="B93" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C93" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C93" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="94">
@@ -10533,10 +10578,10 @@
         <v>46046.068173912034</v>
       </c>
       <c r="B94" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C94" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C94" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="95">
@@ -10544,10 +10589,10 @@
         <v>46046.06818884259</v>
       </c>
       <c r="B95" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C95" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C95" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="96">
@@ -10555,10 +10600,10 @@
         <v>46046.06822234954</v>
       </c>
       <c r="B96" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C96" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C96" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="97">
@@ -10566,10 +10611,10 @@
         <v>46046.06827836805</v>
       </c>
       <c r="B97" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C97" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="98">
@@ -10577,10 +10622,10 @@
         <v>46046.068321377315</v>
       </c>
       <c r="B98" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C98" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C98" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="99">
@@ -10588,10 +10633,10 @@
         <v>46046.06835361111</v>
       </c>
       <c r="B99" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C99" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C99" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="100">
@@ -10599,10 +10644,10 @@
         <v>46046.06860412037</v>
       </c>
       <c r="B100" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C100" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="101">
@@ -10610,10 +10655,10 @@
         <v>46046.06863541667</v>
       </c>
       <c r="B101" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C101" s="22" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="102">
@@ -10621,10 +10666,10 @@
         <v>46046.068643900464</v>
       </c>
       <c r="B102" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C102" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C102" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="103">
@@ -10632,10 +10677,10 @@
         <v>46046.0686666088</v>
       </c>
       <c r="B103" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C103" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C103" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="104">
@@ -10643,10 +10688,10 @@
         <v>46046.068680613425</v>
       </c>
       <c r="B104" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C104" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C104" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="105">
@@ -10654,10 +10699,10 @@
         <v>46046.06868881945</v>
       </c>
       <c r="B105" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C105" s="22" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="106">
@@ -10665,10 +10710,10 @@
         <v>46046.068707094906</v>
       </c>
       <c r="B106" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C106" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C106" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="107">
@@ -10676,10 +10721,10 @@
         <v>46046.068716932874</v>
       </c>
       <c r="B107" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C107" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C107" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="108">
@@ -10687,10 +10732,10 @@
         <v>46046.06875846065</v>
       </c>
       <c r="B108" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C108" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C108" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="109">
@@ -10698,10 +10743,10 @@
         <v>46046.06937510417</v>
       </c>
       <c r="B109" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C109" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C109" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="110">
@@ -10709,10 +10754,10 @@
         <v>46046.06941165509</v>
       </c>
       <c r="B110" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C110" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C110" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="111">
@@ -10720,10 +10765,10 @@
         <v>46046.07081366898</v>
       </c>
       <c r="B111" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C111" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C111" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="112">
@@ -10731,10 +10776,10 @@
         <v>46046.07085496528</v>
       </c>
       <c r="B112" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C112" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C112" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="113">
@@ -10742,10 +10787,10 @@
         <v>46046.070969884255</v>
       </c>
       <c r="B113" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C113" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C113" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="114">
@@ -10753,10 +10798,10 @@
         <v>46046.071016064816</v>
       </c>
       <c r="B114" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C114" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C114" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="115">
@@ -10764,10 +10809,10 @@
         <v>46046.07177228009</v>
       </c>
       <c r="B115" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C115" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C115" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="116">
@@ -10775,10 +10820,10 @@
         <v>46046.07182628472</v>
       </c>
       <c r="B116" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C116" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C116" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="117">
@@ -10786,10 +10831,10 @@
         <v>46046.07194034722</v>
       </c>
       <c r="B117" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C117" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C117" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="118">
@@ -10797,10 +10842,10 @@
         <v>46046.0719809375</v>
       </c>
       <c r="B118" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C118" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C118" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="119">
@@ -10808,10 +10853,10 @@
         <v>46046.072018969906</v>
       </c>
       <c r="B119" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C119" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C119" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="120">
@@ -10819,10 +10864,10 @@
         <v>46046.07205640046</v>
       </c>
       <c r="B120" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C120" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C120" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="121">
@@ -10830,10 +10875,10 @@
         <v>46046.07208803241</v>
       </c>
       <c r="B121" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C121" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="122">
@@ -10841,10 +10886,10 @@
         <v>46046.07213054398</v>
       </c>
       <c r="B122" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C122" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C122" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="123">
@@ -10852,10 +10897,10 @@
         <v>46046.07218134259</v>
       </c>
       <c r="B123" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C123" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C123" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="124">
@@ -10863,10 +10908,10 @@
         <v>46046.072380011574</v>
       </c>
       <c r="B124" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C124" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C124" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="125">
@@ -10874,10 +10919,10 @@
         <v>46046.072436030096</v>
       </c>
       <c r="B125" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C125" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C125" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="126">
@@ -10885,10 +10930,10 @@
         <v>46046.07246744213</v>
       </c>
       <c r="B126" s="22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C126" s="22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="127">
@@ -10896,10 +10941,10 @@
         <v>46046.072472106476</v>
       </c>
       <c r="B127" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C127" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="128">
@@ -10907,10 +10952,10 @@
         <v>46046.07250163195</v>
       </c>
       <c r="B128" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C128" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C128" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="129">
@@ -10918,10 +10963,10 @@
         <v>46046.07254190972</v>
       </c>
       <c r="B129" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C129" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C129" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="130">
@@ -10929,10 +10974,10 @@
         <v>46046.072808067125</v>
       </c>
       <c r="B130" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C130" s="22" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="131">
@@ -10940,10 +10985,10 @@
         <v>46046.072843738424</v>
       </c>
       <c r="B131" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C131" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C131" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="132">
@@ -10951,10 +10996,10 @@
         <v>46046.07285586806</v>
       </c>
       <c r="B132" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C132" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C132" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="133">
@@ -10962,10 +11007,10 @@
         <v>46046.07289621528</v>
       </c>
       <c r="B133" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C133" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C133" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="134">
@@ -10973,10 +11018,10 @@
         <v>46046.0759215162</v>
       </c>
       <c r="B134" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C134" s="22" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="135">
@@ -10984,10 +11029,10 @@
         <v>46046.07595625</v>
       </c>
       <c r="B135" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C135" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C135" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="136">
@@ -10995,10 +11040,10 @@
         <v>46046.07599045139</v>
       </c>
       <c r="B136" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C136" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C136" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="137">
@@ -11006,10 +11051,10 @@
         <v>46046.07603457176</v>
       </c>
       <c r="B137" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C137" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C137" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="138">
@@ -11017,10 +11062,10 @@
         <v>46046.08023099537</v>
       </c>
       <c r="B138" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C138" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C138" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="139">
@@ -11028,10 +11073,10 @@
         <v>46046.0802716551</v>
       </c>
       <c r="B139" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C139" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C139" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="140">
@@ -11039,10 +11084,10 @@
         <v>46046.08028930555</v>
       </c>
       <c r="B140" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C140" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="141">
@@ -11050,10 +11095,10 @@
         <v>46046.08031974537</v>
       </c>
       <c r="B141" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C141" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C141" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="142">
@@ -11061,10 +11106,10 @@
         <v>46046.08036241899</v>
       </c>
       <c r="B142" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C142" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C142" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="143">
@@ -11072,10 +11117,10 @@
         <v>46046.08045652778</v>
       </c>
       <c r="B143" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C143" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C143" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="144">
@@ -11083,10 +11128,10 @@
         <v>46046.08050532408</v>
       </c>
       <c r="B144" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C144" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C144" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="145">
@@ -11094,10 +11139,10 @@
         <v>46046.080519386574</v>
       </c>
       <c r="B145" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C145" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="146">
@@ -11105,10 +11150,10 @@
         <v>46046.08055662037</v>
       </c>
       <c r="B146" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C146" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C146" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="147">
@@ -11116,10 +11161,10 @@
         <v>46046.08060408565</v>
       </c>
       <c r="B147" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C147" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C147" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="148">
@@ -11127,10 +11172,10 @@
         <v>46046.08096555556</v>
       </c>
       <c r="B148" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C148" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C148" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="149">
@@ -11138,10 +11183,10 @@
         <v>46046.08102085648</v>
       </c>
       <c r="B149" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C149" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="150">
@@ -11149,10 +11194,10 @@
         <v>46046.08103068287</v>
       </c>
       <c r="B150" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C150" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C150" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="151">
@@ -11160,10 +11205,10 @@
         <v>46046.08107806713</v>
       </c>
       <c r="B151" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C151" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C151" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="152">
@@ -11171,10 +11216,10 @@
         <v>46046.08111215278</v>
       </c>
       <c r="B152" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C152" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C152" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="153">
@@ -11182,10 +11227,10 @@
         <v>46046.082529618056</v>
       </c>
       <c r="B153" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C153" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C153" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="154">
@@ -11193,10 +11238,10 @@
         <v>46046.082576030094</v>
       </c>
       <c r="B154" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C154" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C154" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="155">
@@ -11204,10 +11249,10 @@
         <v>46046.08258716435</v>
       </c>
       <c r="B155" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C155" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="156">
@@ -11215,10 +11260,10 @@
         <v>46046.08262971065</v>
       </c>
       <c r="B156" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C156" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C156" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="157">
@@ -11226,10 +11271,10 @@
         <v>46046.08266778935</v>
       </c>
       <c r="B157" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C157" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C157" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="158">
@@ -11237,10 +11282,10 @@
         <v>46046.08610806713</v>
       </c>
       <c r="B158" s="22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C158" s="22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="159">
@@ -11248,10 +11293,10 @@
         <v>46046.08803665509</v>
       </c>
       <c r="B159" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C159" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C159" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="160">
@@ -11259,10 +11304,10 @@
         <v>46046.08809237268</v>
       </c>
       <c r="B160" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C160" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C160" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="161">
@@ -11270,10 +11315,10 @@
         <v>46046.08811196759</v>
       </c>
       <c r="B161" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C161" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="162">
@@ -11281,10 +11326,10 @@
         <v>46046.08814864584</v>
       </c>
       <c r="B162" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C162" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C162" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="163">
@@ -11292,10 +11337,10 @@
         <v>46046.0881877662</v>
       </c>
       <c r="B163" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C163" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C163" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="164">
@@ -11303,10 +11348,10 @@
         <v>46046.08830310185</v>
       </c>
       <c r="B164" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C164" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C164" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="165">
@@ -11314,10 +11359,10 @@
         <v>46046.088345543976</v>
       </c>
       <c r="B165" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C165" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C165" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="166">
@@ -11325,10 +11370,10 @@
         <v>46046.09080931713</v>
       </c>
       <c r="B166" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C166" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C166" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="167">
@@ -11336,10 +11381,10 @@
         <v>46046.09084388889</v>
       </c>
       <c r="B167" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C167" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C167" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="168">
@@ -11347,10 +11392,10 @@
         <v>46046.090915416666</v>
       </c>
       <c r="B168" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C168" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="169">
@@ -11358,10 +11403,10 @@
         <v>46046.09095010417</v>
       </c>
       <c r="B169" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C169" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C169" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="170">
@@ -11369,10 +11414,10 @@
         <v>46046.0909856713</v>
       </c>
       <c r="B170" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C170" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C170" s="22" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="171">
@@ -11380,10 +11425,10 @@
         <v>46046.091297129635</v>
       </c>
       <c r="B171" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C171" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="172">
@@ -11391,10 +11436,10 @@
         <v>46046.09133760417</v>
       </c>
       <c r="B172" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C172" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C172" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="173">
@@ -11402,419 +11447,1507 @@
         <v>46046.09137521991</v>
       </c>
       <c r="B173" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C173" s="22" t="s">
         <v>222</v>
       </c>
-      <c r="C173" s="22" t="s">
-        <v>223</v>
-      </c>
     </row>
     <row r="174">
-      <c r="A174" s="25"/>
+      <c r="A174" s="25">
+        <v>46046.09243395833</v>
+      </c>
+      <c r="B174" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C174" s="22" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="175">
-      <c r="A175" s="25"/>
+      <c r="A175" s="25">
+        <v>46046.092955706015</v>
+      </c>
+      <c r="B175" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C175" s="22" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="176">
-      <c r="A176" s="25"/>
+      <c r="A176" s="25">
+        <v>46046.092962662035</v>
+      </c>
+      <c r="B176" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="C176" s="22" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="177">
-      <c r="A177" s="25"/>
+      <c r="A177" s="25">
+        <v>46046.093125300926</v>
+      </c>
+      <c r="B177" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C177" s="22" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="178">
-      <c r="A178" s="25"/>
+      <c r="A178" s="25">
+        <v>46046.09320295139</v>
+      </c>
+      <c r="B178" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C178" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="179">
-      <c r="A179" s="25"/>
+      <c r="A179" s="25">
+        <v>46046.0932903125</v>
+      </c>
+      <c r="B179" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C179" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="180">
-      <c r="A180" s="25"/>
+      <c r="A180" s="25">
+        <v>46046.09337902778</v>
+      </c>
+      <c r="B180" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C180" s="22" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="181">
-      <c r="A181" s="25"/>
+      <c r="A181" s="25">
+        <v>46046.093383217594</v>
+      </c>
+      <c r="B181" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="C181" s="22" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="182">
-      <c r="A182" s="25"/>
+      <c r="A182" s="25">
+        <v>46046.093492025466</v>
+      </c>
+      <c r="B182" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C182" s="22" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="183">
-      <c r="A183" s="25"/>
+      <c r="A183" s="25">
+        <v>46046.095237534726</v>
+      </c>
+      <c r="B183" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C183" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="184">
-      <c r="A184" s="25"/>
+      <c r="A184" s="25">
+        <v>46046.09527609954</v>
+      </c>
+      <c r="B184" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C184" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="185">
-      <c r="A185" s="25"/>
+      <c r="A185" s="25">
+        <v>46046.09530918981</v>
+      </c>
+      <c r="B185" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C185" s="22" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="186">
-      <c r="A186" s="25"/>
+      <c r="A186" s="25">
+        <v>46046.09534825232</v>
+      </c>
+      <c r="B186" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C186" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="187">
-      <c r="A187" s="25"/>
+      <c r="A187" s="25">
+        <v>46046.095401597224</v>
+      </c>
+      <c r="B187" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C187" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="188">
-      <c r="A188" s="25"/>
+      <c r="A188" s="25">
+        <v>46046.095638425926</v>
+      </c>
+      <c r="B188" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C188" s="22" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="189">
-      <c r="A189" s="25"/>
+      <c r="A189" s="25">
+        <v>46046.09566878472</v>
+      </c>
+      <c r="B189" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C189" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="190">
-      <c r="A190" s="25"/>
+      <c r="A190" s="25">
+        <v>46046.09571349537</v>
+      </c>
+      <c r="B190" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C190" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="191">
-      <c r="A191" s="25"/>
+      <c r="A191" s="25">
+        <v>46046.09616177084</v>
+      </c>
+      <c r="B191" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C191" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="192">
-      <c r="A192" s="25"/>
+      <c r="A192" s="25">
+        <v>46046.09641209491</v>
+      </c>
+      <c r="B192" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C192" s="22" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="193">
-      <c r="A193" s="25"/>
+      <c r="A193" s="25">
+        <v>46046.09712612268</v>
+      </c>
+      <c r="B193" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C193" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="194">
-      <c r="A194" s="25"/>
+      <c r="A194" s="25">
+        <v>46046.097161655096</v>
+      </c>
+      <c r="B194" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C194" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="195">
-      <c r="A195" s="25"/>
+      <c r="A195" s="25">
+        <v>46046.0972055787</v>
+      </c>
+      <c r="B195" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C195" s="22" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="196">
-      <c r="A196" s="25"/>
+      <c r="A196" s="25">
+        <v>46046.09725456018</v>
+      </c>
+      <c r="B196" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C196" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="197">
-      <c r="A197" s="25"/>
+      <c r="A197" s="25">
+        <v>46046.09729697916</v>
+      </c>
+      <c r="B197" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C197" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="198">
-      <c r="A198" s="25"/>
+      <c r="A198" s="25">
+        <v>46046.09743432871</v>
+      </c>
+      <c r="B198" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C198" s="22" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="199">
-      <c r="A199" s="25"/>
+      <c r="A199" s="25">
+        <v>46046.097466817126</v>
+      </c>
+      <c r="B199" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C199" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="200">
-      <c r="A200" s="25"/>
+      <c r="A200" s="25">
+        <v>46046.097514594905</v>
+      </c>
+      <c r="B200" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C200" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="201">
-      <c r="A201" s="25"/>
+      <c r="A201" s="25">
+        <v>46046.09895092592</v>
+      </c>
+      <c r="B201" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C201" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="202">
-      <c r="A202" s="25"/>
+      <c r="A202" s="25">
+        <v>46046.098989363425</v>
+      </c>
+      <c r="B202" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C202" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="203">
-      <c r="A203" s="25"/>
+      <c r="A203" s="25">
+        <v>46046.09901777778</v>
+      </c>
+      <c r="B203" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C203" s="22" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="204">
-      <c r="A204" s="25"/>
+      <c r="A204" s="25">
+        <v>46046.09905188657</v>
+      </c>
+      <c r="B204" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C204" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="205">
-      <c r="A205" s="25"/>
+      <c r="A205" s="25">
+        <v>46046.0990971412</v>
+      </c>
+      <c r="B205" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C205" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="206">
-      <c r="A206" s="25"/>
+      <c r="A206" s="25">
+        <v>46046.09925457176</v>
+      </c>
+      <c r="B206" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C206" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="207">
-      <c r="A207" s="25"/>
+      <c r="A207" s="25">
+        <v>46046.09930210648</v>
+      </c>
+      <c r="B207" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C207" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="208">
-      <c r="A208" s="25"/>
+      <c r="A208" s="25">
+        <v>46046.09932429398</v>
+      </c>
+      <c r="B208" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C208" s="22" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="209">
-      <c r="A209" s="25"/>
+      <c r="A209" s="25">
+        <v>46046.099373310186</v>
+      </c>
+      <c r="B209" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C209" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="210">
-      <c r="A210" s="25"/>
+      <c r="A210" s="25">
+        <v>46046.09944068287</v>
+      </c>
+      <c r="B210" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C210" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="211">
-      <c r="A211" s="25"/>
+      <c r="A211" s="25">
+        <v>46046.099836574074</v>
+      </c>
+      <c r="B211" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C211" s="22" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="212">
-      <c r="A212" s="25"/>
+      <c r="A212" s="25">
+        <v>46046.0998650463</v>
+      </c>
+      <c r="B212" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C212" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="213">
-      <c r="A213" s="25"/>
+      <c r="A213" s="25">
+        <v>46046.09990554398</v>
+      </c>
+      <c r="B213" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C213" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="214">
-      <c r="A214" s="25"/>
+      <c r="A214" s="25">
+        <v>46046.10005075231</v>
+      </c>
+      <c r="B214" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C214" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="215">
-      <c r="A215" s="25"/>
+      <c r="A215" s="25">
+        <v>46046.100096678245</v>
+      </c>
+      <c r="B215" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C215" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="216">
-      <c r="A216" s="25"/>
+      <c r="A216" s="25">
+        <v>46046.10059232639</v>
+      </c>
+      <c r="B216" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C216" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="217">
-      <c r="A217" s="25"/>
+      <c r="A217" s="25">
+        <v>46046.100648935186</v>
+      </c>
+      <c r="B217" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C217" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="218">
-      <c r="A218" s="25"/>
+      <c r="A218" s="25">
+        <v>46046.101204606486</v>
+      </c>
+      <c r="B218" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C218" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="219">
-      <c r="A219" s="25"/>
+      <c r="A219" s="25">
+        <v>46046.10141564815</v>
+      </c>
+      <c r="B219" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C219" s="22" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="220">
-      <c r="A220" s="25"/>
+      <c r="A220" s="25">
+        <v>46046.101420590276</v>
+      </c>
+      <c r="B220" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="C220" s="22" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="221">
-      <c r="A221" s="25"/>
+      <c r="A221" s="25">
+        <v>46046.101590624996</v>
+      </c>
+      <c r="B221" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C221" s="22" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="222">
-      <c r="A222" s="25"/>
+      <c r="A222" s="25">
+        <v>46046.10174621528</v>
+      </c>
+      <c r="B222" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C222" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="223">
-      <c r="A223" s="25"/>
+      <c r="A223" s="25">
+        <v>46046.104571296295</v>
+      </c>
+      <c r="B223" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C223" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="224">
-      <c r="A224" s="25"/>
+      <c r="A224" s="25">
+        <v>46046.104608344904</v>
+      </c>
+      <c r="B224" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C224" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="225">
-      <c r="A225" s="25"/>
+      <c r="A225" s="25">
+        <v>46046.104732754626</v>
+      </c>
+      <c r="B225" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C225" s="22" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="226">
-      <c r="A226" s="25"/>
+      <c r="A226" s="25">
+        <v>46046.10477119213</v>
+      </c>
+      <c r="B226" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C226" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="227">
-      <c r="A227" s="25"/>
+      <c r="A227" s="25">
+        <v>46046.10481078704</v>
+      </c>
+      <c r="B227" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C227" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="228">
-      <c r="A228" s="25"/>
+      <c r="A228" s="25">
+        <v>46046.10486158565</v>
+      </c>
+      <c r="B228" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C228" s="22" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="229">
-      <c r="A229" s="25"/>
+      <c r="A229" s="25">
+        <v>46046.10489104167</v>
+      </c>
+      <c r="B229" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C229" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="230">
-      <c r="A230" s="25"/>
+      <c r="A230" s="25">
+        <v>46046.10492611111</v>
+      </c>
+      <c r="B230" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C230" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="231">
-      <c r="A231" s="25"/>
+      <c r="A231" s="25">
+        <v>46046.10576561342</v>
+      </c>
+      <c r="B231" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C231" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="232">
-      <c r="A232" s="25"/>
+      <c r="A232" s="25">
+        <v>46046.10581483797</v>
+      </c>
+      <c r="B232" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C232" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="233">
-      <c r="A233" s="25"/>
+      <c r="A233" s="25">
+        <v>46046.10694038194</v>
+      </c>
+      <c r="B233" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C233" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="234">
-      <c r="A234" s="25"/>
+      <c r="A234" s="25">
+        <v>46046.106977476855</v>
+      </c>
+      <c r="B234" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C234" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="235">
-      <c r="A235" s="25"/>
+      <c r="A235" s="25">
+        <v>46046.10749155092</v>
+      </c>
+      <c r="B235" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C235" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="236">
-      <c r="A236" s="25"/>
+      <c r="A236" s="25">
+        <v>46046.107535891206</v>
+      </c>
+      <c r="B236" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C236" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="237">
-      <c r="A237" s="25"/>
+      <c r="A237" s="25">
+        <v>46046.10754803241</v>
+      </c>
+      <c r="B237" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C237" s="22" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="238">
-      <c r="A238" s="25"/>
+      <c r="A238" s="25">
+        <v>46046.107583425925</v>
+      </c>
+      <c r="B238" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C238" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="239">
-      <c r="A239" s="25"/>
+      <c r="A239" s="25">
+        <v>46046.10762747686</v>
+      </c>
+      <c r="B239" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C239" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="240">
-      <c r="A240" s="25"/>
+      <c r="A240" s="25">
+        <v>46046.107638692134</v>
+      </c>
+      <c r="B240" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C240" s="22" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="241">
-      <c r="A241" s="25"/>
+      <c r="A241" s="25">
+        <v>46046.10766751158</v>
+      </c>
+      <c r="B241" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C241" s="22" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="242">
-      <c r="A242" s="25"/>
+      <c r="A242" s="25">
+        <v>46046.107669930556</v>
+      </c>
+      <c r="B242" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C242" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="243">
-      <c r="A243" s="25"/>
+      <c r="A243" s="25">
+        <v>46046.107687662035</v>
+      </c>
+      <c r="B243" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C243" s="22" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="244">
-      <c r="A244" s="25"/>
+      <c r="A244" s="25">
+        <v>46046.107695370374</v>
+      </c>
+      <c r="B244" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C244" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="245">
-      <c r="A245" s="25"/>
+      <c r="A245" s="25">
+        <v>46046.10770658565</v>
+      </c>
+      <c r="B245" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C245" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="246">
-      <c r="A246" s="25"/>
+      <c r="A246" s="25">
+        <v>46046.10772501158</v>
+      </c>
+      <c r="B246" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C246" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="247">
-      <c r="A247" s="25"/>
+      <c r="A247" s="25">
+        <v>46046.10772486111</v>
+      </c>
+      <c r="B247" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C247" s="22" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="248">
-      <c r="A248" s="25"/>
+      <c r="A248" s="25">
+        <v>46046.1077362963</v>
+      </c>
+      <c r="B248" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C248" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="249">
-      <c r="A249" s="25"/>
+      <c r="A249" s="25">
+        <v>46046.10775667824</v>
+      </c>
+      <c r="B249" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C249" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="250">
-      <c r="A250" s="25"/>
+      <c r="A250" s="25">
+        <v>46046.107762291664</v>
+      </c>
+      <c r="B250" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C250" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="251">
-      <c r="A251" s="25"/>
+      <c r="A251" s="25">
+        <v>46046.10779497685</v>
+      </c>
+      <c r="B251" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C251" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="252">
-      <c r="A252" s="25"/>
+      <c r="A252" s="25">
+        <v>46046.10781126157</v>
+      </c>
+      <c r="B252" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C252" s="22" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="253">
-      <c r="A253" s="25"/>
+      <c r="A253" s="25">
+        <v>46046.10784399306</v>
+      </c>
+      <c r="B253" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C253" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="254">
-      <c r="A254" s="25"/>
+      <c r="A254" s="25">
+        <v>46046.10786568287</v>
+      </c>
+      <c r="B254" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C254" s="22" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="255">
-      <c r="A255" s="25"/>
+      <c r="A255" s="25">
+        <v>46046.10788222222</v>
+      </c>
+      <c r="B255" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C255" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="256">
-      <c r="A256" s="25"/>
+      <c r="A256" s="25">
+        <v>46046.10788855324</v>
+      </c>
+      <c r="B256" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C256" s="22" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="257">
-      <c r="A257" s="25"/>
+      <c r="A257" s="25">
+        <v>46046.107894201385</v>
+      </c>
+      <c r="B257" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C257" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="258">
-      <c r="A258" s="25"/>
+      <c r="A258" s="25">
+        <v>46046.10791181713</v>
+      </c>
+      <c r="B258" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C258" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="259">
-      <c r="A259" s="25"/>
+      <c r="A259" s="25">
+        <v>46046.10791075231</v>
+      </c>
+      <c r="B259" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C259" s="22" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="260">
-      <c r="A260" s="25"/>
+      <c r="A260" s="25">
+        <v>46046.10793436343</v>
+      </c>
+      <c r="B260" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C260" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="261">
-      <c r="A261" s="25"/>
+      <c r="A261" s="25">
+        <v>46046.107955983796</v>
+      </c>
+      <c r="B261" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C261" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="262">
-      <c r="A262" s="25"/>
+      <c r="A262" s="25">
+        <v>46046.1079578125</v>
+      </c>
+      <c r="B262" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C262" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="263">
-      <c r="A263" s="25"/>
+      <c r="A263" s="25">
+        <v>46046.10800129629</v>
+      </c>
+      <c r="B263" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C263" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="264">
-      <c r="A264" s="25"/>
+      <c r="A264" s="25">
+        <v>46046.108041087966</v>
+      </c>
+      <c r="B264" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C264" s="22" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="265">
-      <c r="A265" s="25"/>
+      <c r="A265" s="25">
+        <v>46046.10807944444</v>
+      </c>
+      <c r="B265" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C265" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="266">
-      <c r="A266" s="25"/>
+      <c r="A266" s="25">
+        <v>46046.1081178125</v>
+      </c>
+      <c r="B266" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C266" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="267">
-      <c r="A267" s="25"/>
+      <c r="A267" s="25">
+        <v>46046.108125300925</v>
+      </c>
+      <c r="B267" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C267" s="22" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="268">
-      <c r="A268" s="25"/>
+      <c r="A268" s="25">
+        <v>46046.108158020834</v>
+      </c>
+      <c r="B268" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C268" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="269">
-      <c r="A269" s="25"/>
+      <c r="A269" s="25">
+        <v>46046.10819104167</v>
+      </c>
+      <c r="B269" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C269" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="270">
-      <c r="A270" s="25"/>
+      <c r="A270" s="25">
+        <v>46046.10820520834</v>
+      </c>
+      <c r="B270" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C270" s="22" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="271">
-      <c r="A271" s="25"/>
+      <c r="A271" s="25">
+        <v>46046.108251157406</v>
+      </c>
+      <c r="B271" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C271" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="272">
-      <c r="A272" s="25"/>
+      <c r="A272" s="25">
+        <v>46046.10828569444</v>
+      </c>
+      <c r="B272" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C272" s="22" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="273">
-      <c r="A273" s="25"/>
+      <c r="A273" s="25">
+        <v>46046.10831108796</v>
+      </c>
+      <c r="B273" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C273" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="274">
-      <c r="A274" s="25"/>
+      <c r="A274" s="25">
+        <v>46046.10831696759</v>
+      </c>
+      <c r="B274" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C274" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="275">
-      <c r="A275" s="25"/>
+      <c r="A275" s="25">
+        <v>46046.10836594907</v>
+      </c>
+      <c r="B275" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C275" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="276">
-      <c r="A276" s="25"/>
+      <c r="A276" s="25">
+        <v>46046.10839689815</v>
+      </c>
+      <c r="B276" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C276" s="22" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="277">
-      <c r="A277" s="25"/>
+      <c r="A277" s="25">
+        <v>46046.10842614583</v>
+      </c>
+      <c r="B277" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C277" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="278">
-      <c r="A278" s="25"/>
+      <c r="A278" s="25">
+        <v>46046.10847011574</v>
+      </c>
+      <c r="B278" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C278" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="279">
-      <c r="A279" s="25"/>
+      <c r="A279" s="25">
+        <v>46046.10849130787</v>
+      </c>
+      <c r="B279" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C279" s="22" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="280">
-      <c r="A280" s="25"/>
+      <c r="A280" s="25">
+        <v>46046.10852076389</v>
+      </c>
+      <c r="B280" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C280" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="281">
-      <c r="A281" s="25"/>
+      <c r="A281" s="25">
+        <v>46046.10855888889</v>
+      </c>
+      <c r="B281" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C281" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="282">
-      <c r="A282" s="25"/>
+      <c r="A282" s="25">
+        <v>46046.10857846065</v>
+      </c>
+      <c r="B282" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C282" s="22" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="283">
-      <c r="A283" s="25"/>
+      <c r="A283" s="25">
+        <v>46046.10860466435</v>
+      </c>
+      <c r="B283" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C283" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="284">
-      <c r="A284" s="25"/>
+      <c r="A284" s="25">
+        <v>46046.1086444213</v>
+      </c>
+      <c r="B284" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C284" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="285">
-      <c r="A285" s="25"/>
+      <c r="A285" s="25">
+        <v>46046.10874098379</v>
+      </c>
+      <c r="B285" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C285" s="22" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="286">
-      <c r="A286" s="25"/>
+      <c r="A286" s="25">
+        <v>46046.108771342595</v>
+      </c>
+      <c r="B286" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C286" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="287">
-      <c r="A287" s="25"/>
+      <c r="A287" s="25">
+        <v>46046.108815775464</v>
+      </c>
+      <c r="B287" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C287" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="288">
-      <c r="A288" s="25"/>
+      <c r="A288" s="25">
+        <v>46046.10907377314</v>
+      </c>
+      <c r="B288" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C288" s="22" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="289">
-      <c r="A289" s="25"/>
+      <c r="A289" s="25">
+        <v>46046.1091069213</v>
+      </c>
+      <c r="B289" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C289" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="290">
-      <c r="A290" s="25"/>
+      <c r="A290" s="25">
+        <v>46046.10911388889</v>
+      </c>
+      <c r="B290" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C290" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="291">
-      <c r="A291" s="25"/>
+      <c r="A291" s="25">
+        <v>46046.10915472222</v>
+      </c>
+      <c r="B291" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C291" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="292">
-      <c r="A292" s="25"/>
+      <c r="A292" s="25">
+        <v>46046.109232222225</v>
+      </c>
+      <c r="B292" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C292" s="22" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="293">
-      <c r="A293" s="25"/>
+      <c r="A293" s="25">
+        <v>46046.10926273148</v>
+      </c>
+      <c r="B293" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C293" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="294">
-      <c r="A294" s="25"/>
+      <c r="A294" s="25">
+        <v>46046.10930556713</v>
+      </c>
+      <c r="B294" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C294" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="295">
-      <c r="A295" s="25"/>
+      <c r="A295" s="25">
+        <v>46046.11115868056</v>
+      </c>
+      <c r="B295" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C295" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="296">
-      <c r="A296" s="25"/>
+      <c r="A296" s="25">
+        <v>46046.11120475695</v>
+      </c>
+      <c r="B296" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C296" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="297">
-      <c r="A297" s="25"/>
+      <c r="A297" s="25">
+        <v>46046.111265162035</v>
+      </c>
+      <c r="B297" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C297" s="22" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="298">
-      <c r="A298" s="25"/>
+      <c r="A298" s="25">
+        <v>46046.11129320602</v>
+      </c>
+      <c r="B298" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C298" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="299">
-      <c r="A299" s="25"/>
+      <c r="A299" s="25">
+        <v>46046.11133587963</v>
+      </c>
+      <c r="B299" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C299" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="300">
-      <c r="A300" s="25"/>
+      <c r="A300" s="25">
+        <v>46046.11139116898</v>
+      </c>
+      <c r="B300" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C300" s="22" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="301">
-      <c r="A301" s="25"/>
+      <c r="A301" s="25">
+        <v>46046.11143186342</v>
+      </c>
+      <c r="B301" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C301" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="302">
-      <c r="A302" s="25"/>
+      <c r="A302" s="25">
+        <v>46046.111444814815</v>
+      </c>
+      <c r="B302" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C302" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="303">
-      <c r="A303" s="25"/>
+      <c r="A303" s="25">
+        <v>46046.11149435185</v>
+      </c>
+      <c r="B303" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C303" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="304">
-      <c r="A304" s="25"/>
+      <c r="A304" s="25">
+        <v>46046.11171914352</v>
+      </c>
+      <c r="B304" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C304" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="305">
-      <c r="A305" s="25"/>
+      <c r="A305" s="25">
+        <v>46046.111766030095</v>
+      </c>
+      <c r="B305" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C305" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="306">
-      <c r="A306" s="25"/>
+      <c r="A306" s="25">
+        <v>46046.1118228125</v>
+      </c>
+      <c r="B306" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C306" s="22" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="307">
-      <c r="A307" s="25"/>
+      <c r="A307" s="25">
+        <v>46046.11191076389</v>
+      </c>
+      <c r="B307" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C307" s="22" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="308">
-      <c r="A308" s="25"/>
+      <c r="A308" s="25">
+        <v>46046.11194369213</v>
+      </c>
+      <c r="B308" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C308" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="309">
-      <c r="A309" s="25"/>
+      <c r="A309" s="25">
+        <v>46046.111995300926</v>
+      </c>
+      <c r="B309" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C309" s="22" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="310">
       <c r="A310" s="25"/>

</xml_diff>

<commit_message>
fix: update GAS URL to final deployment endpoint in both code and CI config
</commit_message>
<xml_diff>
--- a/商品揭露v2.xlsx
+++ b/商品揭露v2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="241">
   <si>
     <t>WaveID</t>
   </si>
@@ -695,6 +695,9 @@
     <t>POPO</t>
   </si>
   <si>
+    <t>【韓國SAM'S】濟州牛島風味夾心餅(柑橘風味),【Loshi 】馬油保濕乳霜,【LEC超值組】激落君 強力除霉泡泡</t>
+  </si>
+  <si>
     <t>波段</t>
   </si>
   <si>
@@ -744,6 +747,51 @@
   </si>
   <si>
     <t>{"action":"enable_product","wave":"2","leaderId":"Ub6e6a2d6e6358bd68b656638e974b1c6","leaderName":"POPO","prodName":"123","isEnabled":false}</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>DEBUG_Toggle_Started</t>
+  </si>
+  <si>
+    <t>{"prodName":"123","shouldEnable":false,"leaderId":"Ub6e6a2d6e6358bd68b656638e974b1c6","wave":"2","matches":[2]}</t>
+  </si>
+  <si>
+    <t>{"action":"enable_product","wave":"2","leaderId":"Ub6e6a2d6e6358bd68b656638e974b1c6","leaderName":"POPO","prodName":"參虎吃不停爆紅薏仁","isEnabled":true}</t>
+  </si>
+  <si>
+    <t>{"prodName":"參虎吃不停爆紅薏仁","shouldEnable":true,"leaderId":"Ub6e6a2d6e6358bd68b656638e974b1c6","wave":"2","matches":[2]}</t>
+  </si>
+  <si>
+    <t>{"prodName":"123","shouldEnable":true,"leaderId":"Ub6e6a2d6e6358bd68b656638e974b1c6","wave":"2","matches":[2]}</t>
+  </si>
+  <si>
+    <t>{"action":"enable_product","wave":"2","leaderId":"Ub6e6a2d6e6358bd68b656638e974b1c6","leaderName":"POPO","prodName":"【韓國SAM'S】濟州牛島風味夾心餅(柑橘風味)","isEnabled":true}</t>
+  </si>
+  <si>
+    <t>{"prodName":"【韓國SAM'S】濟州牛島風味夾心餅(柑橘風味)","shouldEnable":true,"leaderId":"Ub6e6a2d6e6358bd68b656638e974b1c6","wave":"2","matches":[2]}</t>
+  </si>
+  <si>
+    <t>{"action":"enable_product","wave":"2","leaderId":"Ub6e6a2d6e6358bd68b656638e974b1c6","leaderName":"POPO","prodName":"【Loshi 】馬油保濕乳霜","isEnabled":true}</t>
+  </si>
+  <si>
+    <t>{"prodName":"【Loshi 】馬油保濕乳霜","shouldEnable":true,"leaderId":"Ub6e6a2d6e6358bd68b656638e974b1c6","wave":"2","matches":[2]}</t>
+  </si>
+  <si>
+    <t>{"action":"enable_product","wave":"2","leaderId":"Ub6e6a2d6e6358bd68b656638e974b1c6","leaderName":"POPO","prodName":"【LEC超值組】激落君 強力除霉泡泡","isEnabled":true}</t>
+  </si>
+  <si>
+    <t>{"prodName":"【LEC超值組】激落君 強力除霉泡泡","shouldEnable":true,"leaderId":"Ub6e6a2d6e6358bd68b656638e974b1c6","wave":"2","matches":[2]}</t>
+  </si>
+  <si>
+    <t>{"action":"submit_batch_intent","wave":"2","leaderId":"Ub6e6a2d6e6358bd68b656638e974b1c6","leaderName":"POPO","userId":"Ub6e6a2d6e6358bd68b656638e974b1c6","userName":"POPO","userAvatar":"https://profile.line-scdn.net/0hWc0NtGO9CEwdNxcMGrp2cm1nCyY-RlFeOAQTfysxA3pzUEkeZgRBIiA0UX4hAUYZZVgXfSgyV3g_BQhhLVAAQys0CR9DQi5sURVHT0ZIHR51bCdjRQI4SitTBXlbQkxGWSQGRFhFDiV2XAccawM4d1xrFilTWk55UWBkGhgFZs9yNX8ZMFBOLCA-VX6l","items":[{"prodName":"test2","qty":4}]}</t>
+  </si>
+  <si>
+    <t>{"action":"enable_product","wave":"2","leaderId":"Ub6e6a2d6e6358bd68b656638e974b1c6","leaderName":"POPO","prodName":"參虎吃不停爆紅薏仁","isEnabled":false}</t>
+  </si>
+  <si>
+    <t>{"prodName":"參虎吃不停爆紅薏仁","shouldEnable":false,"leaderId":"Ub6e6a2d6e6358bd68b656638e974b1c6","wave":"2","matches":[2]}</t>
   </si>
 </sst>
 </file>
@@ -7041,7 +7089,7 @@
         <v>46046.12964840278</v>
       </c>
       <c r="G2" s="30" t="s">
-        <v>74</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3">
@@ -11016,30 +11064,30 @@
         <v>198</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>200</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="27" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B2" s="27">
         <v>2.0</v>
@@ -11063,12 +11111,12 @@
         <v>207</v>
       </c>
       <c r="I2" s="32" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="27" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B3" s="27">
         <v>2.0</v>
@@ -11083,21 +11131,21 @@
         <v>195</v>
       </c>
       <c r="F3" s="31">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="G3" s="29">
-        <v>46046.04064731482</v>
+        <v>46046.15036571759</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>207</v>
       </c>
       <c r="I3" s="32" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="27" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B4" s="27">
         <v>2.0</v>
@@ -11121,12 +11169,12 @@
         <v>207</v>
       </c>
       <c r="I4" s="32" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="27" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B5" s="27">
         <v>2.0</v>
@@ -11150,12 +11198,12 @@
         <v>207</v>
       </c>
       <c r="I5" s="32" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="27" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B6" s="27">
         <v>2.0</v>
@@ -11179,7 +11227,7 @@
         <v>207</v>
       </c>
       <c r="I6" s="32" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7">
@@ -11343,8 +11391,8 @@
         <v>test2</v>
       </c>
       <c r="D3" s="35">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
-        <v>1</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5.0)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -11422,13 +11470,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="27" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2">
@@ -11436,10 +11484,10 @@
         <v>46046.12960533565</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3">
@@ -11447,10 +11495,10 @@
         <v>46046.12964398148</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4">
@@ -11458,10 +11506,10 @@
         <v>46046.12982780093</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5">
@@ -11469,10 +11517,10 @@
         <v>46046.129866828705</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6">
@@ -11480,10 +11528,10 @@
         <v>46046.13008859954</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7">
@@ -11491,10 +11539,10 @@
         <v>46046.130119293986</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8">
@@ -11502,10 +11550,10 @@
         <v>46046.13015675926</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9">
@@ -11513,10 +11561,10 @@
         <v>46046.13026414352</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10">
@@ -11524,10 +11572,10 @@
         <v>46046.13029502315</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11">
@@ -11535,284 +11583,1012 @@
         <v>46046.13034145834</v>
       </c>
       <c r="B11" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="29">
+        <v>46046.13110943287</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="29">
+        <v>46046.142816921296</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C13" s="27" t="s">
         <v>221</v>
       </c>
-      <c r="C11" s="27" t="s">
+    </row>
+    <row r="14">
+      <c r="A14" s="29">
+        <v>46046.14285777778</v>
+      </c>
+      <c r="B14" s="27" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="29"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="29"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="29"/>
+      <c r="C14" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="29"/>
+      <c r="A15" s="29">
+        <v>46046.14312298611</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="29"/>
+      <c r="A16" s="29">
+        <v>46046.14315322917</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="29"/>
+      <c r="A17" s="29">
+        <v>46046.143158148145</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="29"/>
+      <c r="A18" s="29">
+        <v>46046.14321864583</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="29"/>
+      <c r="A19" s="29">
+        <v>46046.14322275463</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="29"/>
+      <c r="A20" s="29">
+        <v>46046.14325700232</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" s="29"/>
+      <c r="A21" s="29">
+        <v>46046.143294884256</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" s="29"/>
+      <c r="A22" s="29">
+        <v>46046.145543391205</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" s="29"/>
+      <c r="A23" s="29">
+        <v>46046.1455475463</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" s="29"/>
+      <c r="A24" s="29">
+        <v>46046.14556819445</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" s="29"/>
+      <c r="A25" s="29">
+        <v>46046.14557270834</v>
+      </c>
+      <c r="B25" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="C25" s="27" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" s="29"/>
+      <c r="A26" s="29">
+        <v>46046.14557774305</v>
+      </c>
+      <c r="B26" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" s="29"/>
+      <c r="A27" s="29">
+        <v>46046.145591203705</v>
+      </c>
+      <c r="B27" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C27" s="27" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" s="29"/>
+      <c r="A28" s="29">
+        <v>46046.14559829861</v>
+      </c>
+      <c r="B28" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" s="29"/>
+      <c r="A29" s="29">
+        <v>46046.14560635417</v>
+      </c>
+      <c r="B29" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C29" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" s="29"/>
+      <c r="A30" s="29">
+        <v>46046.145620358795</v>
+      </c>
+      <c r="B30" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C30" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" s="29"/>
+      <c r="A31" s="29">
+        <v>46046.14563506945</v>
+      </c>
+      <c r="B31" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C31" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" s="29"/>
+      <c r="A32" s="29">
+        <v>46046.14565175926</v>
+      </c>
+      <c r="B32" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C32" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" s="29"/>
+      <c r="A33" s="29">
+        <v>46046.145673657404</v>
+      </c>
+      <c r="B33" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C33" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="34">
-      <c r="A34" s="29"/>
+      <c r="A34" s="29">
+        <v>46046.145911354164</v>
+      </c>
+      <c r="B34" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" s="29"/>
+      <c r="A35" s="29">
+        <v>46046.14595868056</v>
+      </c>
+      <c r="B35" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C35" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" s="29"/>
+      <c r="A36" s="29">
+        <v>46046.146582245376</v>
+      </c>
+      <c r="B36" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" s="29"/>
+      <c r="A37" s="29">
+        <v>46046.147221701394</v>
+      </c>
+      <c r="B37" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C37" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" s="29"/>
+      <c r="A38" s="29">
+        <v>46046.14727457176</v>
+      </c>
+      <c r="B38" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C38" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="39">
-      <c r="A39" s="29"/>
+      <c r="A39" s="29">
+        <v>46046.14772115741</v>
+      </c>
+      <c r="B39" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C39" s="27" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="40">
-      <c r="A40" s="29"/>
+      <c r="A40" s="29">
+        <v>46046.14772890046</v>
+      </c>
+      <c r="B40" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="C40" s="27" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="41">
-      <c r="A41" s="29"/>
+      <c r="A41" s="29">
+        <v>46046.14776570602</v>
+      </c>
+      <c r="B41" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C41" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="42">
-      <c r="A42" s="29"/>
+      <c r="A42" s="29">
+        <v>46046.147798148144</v>
+      </c>
+      <c r="B42" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C42" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="43">
-      <c r="A43" s="29"/>
+      <c r="A43" s="29">
+        <v>46046.14831259259</v>
+      </c>
+      <c r="B43" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C43" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="44">
-      <c r="A44" s="29"/>
+      <c r="A44" s="29">
+        <v>46046.148352662036</v>
+      </c>
+      <c r="B44" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C44" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="45">
-      <c r="A45" s="29"/>
+      <c r="A45" s="29">
+        <v>46046.14850267361</v>
+      </c>
+      <c r="B45" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C45" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="46">
-      <c r="A46" s="29"/>
+      <c r="A46" s="29">
+        <v>46046.148555567124</v>
+      </c>
+      <c r="B46" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C46" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="47">
-      <c r="A47" s="29"/>
+      <c r="A47" s="29">
+        <v>46046.148594687504</v>
+      </c>
+      <c r="B47" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C47" s="27" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="48">
-      <c r="A48" s="29"/>
+      <c r="A48" s="29">
+        <v>46046.14860206019</v>
+      </c>
+      <c r="B48" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="C48" s="27" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="49">
-      <c r="A49" s="29"/>
+      <c r="A49" s="29">
+        <v>46046.14863658565</v>
+      </c>
+      <c r="B49" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C49" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="50">
-      <c r="A50" s="29"/>
+      <c r="A50" s="29">
+        <v>46046.1486739699</v>
+      </c>
+      <c r="B50" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C50" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="51">
-      <c r="A51" s="29"/>
+      <c r="A51" s="29">
+        <v>46046.14881097223</v>
+      </c>
+      <c r="B51" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C51" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="52">
-      <c r="A52" s="29"/>
+      <c r="A52" s="29">
+        <v>46046.14885055556</v>
+      </c>
+      <c r="B52" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C52" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="53">
-      <c r="A53" s="29"/>
+      <c r="A53" s="29">
+        <v>46046.1497172338</v>
+      </c>
+      <c r="B53" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C53" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="54">
-      <c r="A54" s="29"/>
+      <c r="A54" s="29">
+        <v>46046.14975378472</v>
+      </c>
+      <c r="B54" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C54" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="55">
-      <c r="A55" s="29"/>
+      <c r="A55" s="29">
+        <v>46046.1499671875</v>
+      </c>
+      <c r="B55" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C55" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="56">
-      <c r="A56" s="29"/>
+      <c r="A56" s="29">
+        <v>46046.150003055554</v>
+      </c>
+      <c r="B56" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C56" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="57">
-      <c r="A57" s="29"/>
+      <c r="A57" s="29">
+        <v>46046.15035527778</v>
+      </c>
+      <c r="B57" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C57" s="27" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="58">
-      <c r="A58" s="29"/>
+      <c r="A58" s="29">
+        <v>46046.15040258101</v>
+      </c>
+      <c r="B58" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C58" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="59">
-      <c r="A59" s="29"/>
+      <c r="A59" s="29">
+        <v>46046.15045065973</v>
+      </c>
+      <c r="B59" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C59" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="60">
-      <c r="A60" s="29"/>
+      <c r="A60" s="29">
+        <v>46046.15377880787</v>
+      </c>
+      <c r="B60" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C60" s="27" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="61">
-      <c r="A61" s="29"/>
+      <c r="A61" s="29">
+        <v>46046.42188361111</v>
+      </c>
+      <c r="B61" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C61" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="62">
-      <c r="A62" s="29"/>
+      <c r="A62" s="29">
+        <v>46046.42193519676</v>
+      </c>
+      <c r="B62" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C62" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="63">
-      <c r="A63" s="29"/>
+      <c r="A63" s="29">
+        <v>46046.42199675926</v>
+      </c>
+      <c r="B63" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C63" s="27" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="64">
-      <c r="A64" s="29"/>
+      <c r="A64" s="29">
+        <v>46046.42200390046</v>
+      </c>
+      <c r="B64" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="C64" s="27" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="65">
-      <c r="A65" s="29"/>
+      <c r="A65" s="29">
+        <v>46046.42203554398</v>
+      </c>
+      <c r="B65" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C65" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="66">
-      <c r="A66" s="29"/>
+      <c r="A66" s="29">
+        <v>46046.42207920139</v>
+      </c>
+      <c r="B66" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C66" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="67">
-      <c r="A67" s="29"/>
+      <c r="A67" s="29">
+        <v>46046.42223148148</v>
+      </c>
+      <c r="B67" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C67" s="27" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="68">
-      <c r="A68" s="29"/>
+      <c r="A68" s="29">
+        <v>46046.42223991898</v>
+      </c>
+      <c r="B68" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="C68" s="27" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="69">
-      <c r="A69" s="29"/>
+      <c r="A69" s="29">
+        <v>46046.42227420139</v>
+      </c>
+      <c r="B69" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C69" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="70">
-      <c r="A70" s="29"/>
+      <c r="A70" s="29">
+        <v>46046.42231164352</v>
+      </c>
+      <c r="B70" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C70" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="71">
-      <c r="A71" s="29"/>
+      <c r="A71" s="29">
+        <v>46046.47740101852</v>
+      </c>
+      <c r="B71" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C71" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="72">
-      <c r="A72" s="29"/>
+      <c r="A72" s="29">
+        <v>46046.477441875</v>
+      </c>
+      <c r="B72" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C72" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="73">
-      <c r="A73" s="29"/>
+      <c r="A73" s="29">
+        <v>46046.48382434028</v>
+      </c>
+      <c r="B73" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C73" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="74">
-      <c r="A74" s="29"/>
+      <c r="A74" s="29">
+        <v>46046.48386655093</v>
+      </c>
+      <c r="B74" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C74" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="75">
-      <c r="A75" s="29"/>
+      <c r="A75" s="29">
+        <v>46046.48398131944</v>
+      </c>
+      <c r="B75" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C75" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="76">
-      <c r="A76" s="29"/>
+      <c r="A76" s="29">
+        <v>46046.48400273148</v>
+      </c>
+      <c r="B76" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C76" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="77">
-      <c r="A77" s="29"/>
+      <c r="A77" s="29">
+        <v>46046.48403920139</v>
+      </c>
+      <c r="B77" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C77" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="78">
-      <c r="A78" s="29"/>
+      <c r="A78" s="29">
+        <v>46046.48417224537</v>
+      </c>
+      <c r="B78" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C78" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="79">
-      <c r="A79" s="29"/>
+      <c r="A79" s="29">
+        <v>46046.484191296295</v>
+      </c>
+      <c r="B79" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C79" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="80">
-      <c r="A80" s="29"/>
+      <c r="A80" s="29">
+        <v>46046.48423299768</v>
+      </c>
+      <c r="B80" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C80" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="81">
-      <c r="A81" s="29"/>
+      <c r="A81" s="29">
+        <v>46046.48430484954</v>
+      </c>
+      <c r="B81" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C81" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="82">
-      <c r="A82" s="29"/>
+      <c r="A82" s="29">
+        <v>46046.48434113426</v>
+      </c>
+      <c r="B82" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C82" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="83">
-      <c r="A83" s="29"/>
+      <c r="A83" s="29">
+        <v>46046.48463017361</v>
+      </c>
+      <c r="B83" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C83" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="84">
-      <c r="A84" s="29"/>
+      <c r="A84" s="29">
+        <v>46046.48468528935</v>
+      </c>
+      <c r="B84" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C84" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="85">
-      <c r="A85" s="29"/>
+      <c r="A85" s="29">
+        <v>46046.48474208333</v>
+      </c>
+      <c r="B85" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C85" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="86">
-      <c r="A86" s="29"/>
+      <c r="A86" s="29">
+        <v>46046.48479743056</v>
+      </c>
+      <c r="B86" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C86" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="87">
-      <c r="A87" s="29"/>
+      <c r="A87" s="29">
+        <v>46046.48514012732</v>
+      </c>
+      <c r="B87" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C87" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="88">
-      <c r="A88" s="29"/>
+      <c r="A88" s="29">
+        <v>46046.485179537034</v>
+      </c>
+      <c r="B88" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C88" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="89">
-      <c r="A89" s="29"/>
+      <c r="A89" s="29">
+        <v>46046.485690057874</v>
+      </c>
+      <c r="B89" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C89" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="90">
-      <c r="A90" s="29"/>
+      <c r="A90" s="29">
+        <v>46046.485745300924</v>
+      </c>
+      <c r="B90" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C90" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="91">
-      <c r="A91" s="29"/>
+      <c r="A91" s="29">
+        <v>46046.5055722338</v>
+      </c>
+      <c r="B91" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C91" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="92">
-      <c r="A92" s="29"/>
+      <c r="A92" s="29">
+        <v>46046.50562210648</v>
+      </c>
+      <c r="B92" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C92" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="93">
-      <c r="A93" s="29"/>
+      <c r="A93" s="29">
+        <v>46046.5057050926</v>
+      </c>
+      <c r="B93" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C93" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="94">
-      <c r="A94" s="29"/>
+      <c r="A94" s="29">
+        <v>46046.505751006946</v>
+      </c>
+      <c r="B94" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C94" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="95">
-      <c r="A95" s="29"/>
+      <c r="A95" s="29">
+        <v>46046.50614935185</v>
+      </c>
+      <c r="B95" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C95" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="96">
-      <c r="A96" s="29"/>
+      <c r="A96" s="29">
+        <v>46046.5061871412</v>
+      </c>
+      <c r="B96" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C96" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="97">
-      <c r="A97" s="29"/>
+      <c r="A97" s="29">
+        <v>46046.506756874995</v>
+      </c>
+      <c r="B97" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C97" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="98">
-      <c r="A98" s="29"/>
+      <c r="A98" s="29">
+        <v>46046.506799571755</v>
+      </c>
+      <c r="B98" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C98" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="99">
-      <c r="A99" s="29"/>
+      <c r="A99" s="29">
+        <v>46046.506972256946</v>
+      </c>
+      <c r="B99" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C99" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="100">
-      <c r="A100" s="29"/>
+      <c r="A100" s="29">
+        <v>46046.50701104167</v>
+      </c>
+      <c r="B100" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C100" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="101">
-      <c r="A101" s="29"/>
+      <c r="A101" s="29">
+        <v>46046.50950865741</v>
+      </c>
+      <c r="B101" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C101" s="27" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="102">
-      <c r="A102" s="29"/>
+      <c r="A102" s="29">
+        <v>46046.50955991898</v>
+      </c>
+      <c r="B102" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C102" s="27" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="29"/>

</xml_diff>